<commit_message>
Cleaned data for weather and survey vars
Added two files. One is the cleaned survey data and the other is the annual city data including global and US data. Updated the data dictionary to add new vars
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\OneDrive\Desktop\GWU\DATS 6103\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c1470ca2a8d9960/Desktop/GWU/DATS 6103/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFB1476-3154-4FAF-B63B-C4744BFFD866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{BFFB1476-3154-4FAF-B63B-C4744BFFD866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C0817B-12EA-478A-A0E6-01676D680888}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="3960" windowWidth="21600" windowHeight="12645" xr2:uid="{EEB60F5F-9775-4871-8FF4-9F0C389910A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EEB60F5F-9775-4871-8FF4-9F0C389910A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
   <si>
     <t>age</t>
   </si>
@@ -200,9 +200,6 @@
     <t>https://sercc.com/noaa-online-weather/</t>
   </si>
   <si>
-    <t>https://www.fema.gov/data-visualization/disaster-declarations-states-and-counties</t>
-  </si>
-  <si>
     <t>FEMA</t>
   </si>
   <si>
@@ -216,6 +213,60 @@
   </si>
   <si>
     <t>9 us regions</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>date of survey</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>marit_status</t>
+  </si>
+  <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>stated religion</t>
+  </si>
+  <si>
+    <t>stated marital status</t>
+  </si>
+  <si>
+    <t>current employment</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>number of children in household</t>
+  </si>
+  <si>
+    <t>number of adults in household</t>
+  </si>
+  <si>
+    <t>Row Mane</t>
+  </si>
+  <si>
+    <t>case_ID</t>
+  </si>
+  <si>
+    <t>research ID to track row</t>
+  </si>
+  <si>
+    <t>https://www.fema.gov/openfema-data-page/public-assistance-funded-projects-details-v1</t>
+  </si>
+  <si>
+    <t>https://www.fema.gov/openfema-data-page/disaster-declarations-summaries-v2</t>
   </si>
 </sst>
 </file>
@@ -596,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330E944E-38E3-4A07-9825-02ABE1356310}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,13 +741,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>44</v>
@@ -958,10 +1009,10 @@
         <v>1000</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -984,10 +1035,10 @@
         <v>1000</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
         <v>55</v>
-      </c>
-      <c r="H16" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,10 +1061,10 @@
         <v>1000</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1066,6 +1117,158 @@
       </c>
       <c r="H19" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>